<commit_message>
shatayuawari: hlookup and documented for v and h lookup
</commit_message>
<xml_diff>
--- a/Day 12.xlsx
+++ b/Day 12.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analytics\Excel\Day 12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659DF93D-50EE-4649-862D-41E56545A7B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C5CAA0-0CEC-4AEB-94DF-1B6414896643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,8 @@
     <sheet name="data types" sheetId="5" r:id="rId5"/>
     <sheet name="Logical" sheetId="6" r:id="rId6"/>
     <sheet name="if_else_if" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet3" sheetId="9" r:id="rId8"/>
-    <sheet name="Sheet4" sheetId="10" r:id="rId9"/>
+    <sheet name="vLookup" sheetId="9" r:id="rId8"/>
+    <sheet name="hLookup" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -439,12 +439,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1469,12 +1469,12 @@
       </c>
     </row>
     <row r="3" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
       <c r="H3" t="s">
         <v>52</v>
       </c>
@@ -1535,11 +1535,11 @@
       </c>
     </row>
     <row r="12" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
       <c r="H12" t="s">
         <v>60</v>
       </c>
@@ -1549,11 +1549,11 @@
       </c>
     </row>
     <row r="13" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
       <c r="H13" t="s">
         <v>61</v>
       </c>
@@ -1568,11 +1568,11 @@
       </c>
     </row>
     <row r="15" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
       <c r="H15" t="s">
         <v>62</v>
       </c>
@@ -1582,11 +1582,11 @@
       </c>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
       <c r="H17" t="s">
         <v>62</v>
       </c>
@@ -1596,11 +1596,11 @@
       </c>
     </row>
     <row r="20" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
       <c r="H20" t="s">
         <v>64</v>
       </c>
@@ -1610,11 +1610,11 @@
       </c>
     </row>
     <row r="22" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
       <c r="H22" t="s">
         <v>65</v>
       </c>
@@ -1624,11 +1624,11 @@
       </c>
     </row>
     <row r="24" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
       <c r="H24" t="s">
         <v>66</v>
       </c>
@@ -1638,21 +1638,21 @@
       </c>
     </row>
     <row r="26" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
       <c r="H26" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="28" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
       <c r="H28" t="s">
         <v>68</v>
       </c>
@@ -1662,33 +1662,33 @@
       </c>
     </row>
     <row r="31" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
       <c r="H31" t="str">
         <f>MID(C31,5,LEN(C31))</f>
         <v>da25 8:35</v>
       </c>
     </row>
     <row r="32" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
       <c r="H32" t="str">
         <f t="shared" ref="H32:H33" si="0">MID(C32,5,LEN(C32))</f>
         <v>da25 in ARC 8:35</v>
       </c>
     </row>
     <row r="33" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C33" s="21" t="s">
+      <c r="C33" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
       <c r="H33" t="str">
         <f t="shared" si="0"/>
         <v>da25 in vigo camp ARC 8:35</v>
@@ -1696,11 +1696,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C17:E17"/>
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="C32:E32"/>
     <mergeCell ref="C33:E33"/>
@@ -1709,6 +1704,11 @@
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="C26:E26"/>
     <mergeCell ref="C28:E28"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2672,16 +2672,16 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E1A0A62-B4DD-4993-8E44-09635BAAAE07}">
-  <dimension ref="C6:I17"/>
+  <dimension ref="B6:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10:I10"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
@@ -2689,209 +2689,254 @@
     <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C6" s="22" t="s">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C6" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="21" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="23" t="s">
+    <row r="7" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="C7" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="23" t="s">
+      <c r="D7" s="23" t="str">
+        <f>HLOOKUP(D6,$C$15:$I$17,2,FALSE)</f>
+        <v>automotive sq, near tp road 40001</v>
+      </c>
+      <c r="E7" s="23" t="str">
+        <f t="shared" ref="E7:I7" si="0">HLOOKUP(E6,$C$15:$I$17,2,FALSE)</f>
+        <v>offline</v>
+      </c>
+      <c r="F7" s="23">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G7" s="23">
+        <f t="shared" si="0"/>
+        <v>5000</v>
+      </c>
+      <c r="H7" s="23">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+      <c r="I7" s="23">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C8" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="22">
         <v>2</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8" s="22">
         <v>1000</v>
       </c>
-      <c r="H8" s="23">
+      <c r="H8" s="22">
         <v>10000</v>
       </c>
-      <c r="I8" s="23">
+      <c r="I8" s="22">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="23" t="s">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="22">
         <v>6</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="22">
         <v>7000</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="22">
         <v>200000</v>
       </c>
-      <c r="I9" s="23">
+      <c r="I9" s="22">
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="23" t="s">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-    </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="23" t="s">
+      <c r="D10" s="22" t="str">
+        <f>HLOOKUP(D6,$C$15:$I$17,3,FALSE)</f>
+        <v>nandanvan</v>
+      </c>
+      <c r="E10" s="22" t="str">
+        <f t="shared" ref="E10:I10" si="1">HLOOKUP(E6,$C$15:$I$17,3,FALSE)</f>
+        <v>online</v>
+      </c>
+      <c r="F10" s="22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G10" s="22">
+        <f t="shared" si="1"/>
+        <v>15000</v>
+      </c>
+      <c r="H10" s="22">
+        <f t="shared" si="1"/>
+        <v>200000</v>
+      </c>
+      <c r="I10" s="22">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C11" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F11" s="22">
         <v>3</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="22">
         <v>12000</v>
       </c>
-      <c r="H11" s="23">
+      <c r="H11" s="22">
         <v>150000</v>
       </c>
-      <c r="I11" s="23">
+      <c r="I11" s="22">
         <v>7000</v>
       </c>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C12" s="23" t="s">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C12" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="22">
         <v>10</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="22">
         <v>2000</v>
       </c>
-      <c r="H12" s="23">
+      <c r="H12" s="22">
         <v>50000</v>
       </c>
-      <c r="I12" s="23">
+      <c r="I12" s="22">
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="22" t="s">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="22" t="s">
+      <c r="H15" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="22" t="s">
+      <c r="I15" s="21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="3:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="C16" s="23" t="s">
+    <row r="16" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="22">
         <v>700</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="22">
         <v>5000</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="22">
         <v>100000</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="23">
+      <c r="H16" s="22">
         <v>5</v>
       </c>
-      <c r="I16" s="24" t="s">
+      <c r="I16" s="23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C17" s="23" t="s">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="22">
         <v>5000</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17" s="22">
         <v>15000</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17" s="22">
         <v>200000</v>
       </c>
-      <c r="G17" s="23" t="s">
+      <c r="G17" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="23">
+      <c r="H17" s="22">
         <v>1</v>
       </c>
-      <c r="I17" s="23" t="s">
+      <c r="I17" s="22" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>